<commit_message>
Testing with test set with both FL and FP models
</commit_message>
<xml_diff>
--- a/Testing.xlsx
+++ b/Testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rishit Thakkar\OneDrive\Desktop\Columbia University\Spring'24\Embedded Systems\Project\MNIST_HW_AXRL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{228FDB5E-C125-4552-9767-FEDD4326C7F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{687B8E85-7A4C-4036-AB0F-48412AA10F0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -624,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3438"/>
+  <dimension ref="A1:J3438"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3419" workbookViewId="0">
-      <selection activeCell="B3438" sqref="B3438"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J340" sqref="J340"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,7 +638,7 @@
     <col min="6" max="6" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -651,8 +651,11 @@
       <c r="F1">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J1">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -665,8 +668,11 @@
       <c r="F2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -679,8 +685,11 @@
       <c r="F3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -693,8 +702,11 @@
       <c r="F4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -707,8 +719,11 @@
       <c r="F5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -721,8 +736,11 @@
       <c r="F6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -735,8 +753,11 @@
       <c r="F7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -749,8 +770,11 @@
       <c r="F8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -763,8 +787,11 @@
       <c r="F9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -777,8 +804,11 @@
       <c r="F10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -791,8 +821,11 @@
       <c r="F11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -805,8 +838,11 @@
       <c r="F12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <v>1.2669E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -819,8 +855,11 @@
       <c r="F13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J13">
+        <v>8.4914000000000003E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -833,8 +872,11 @@
       <c r="F14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <v>0.194329</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -847,8 +889,11 @@
       <c r="F15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J15">
+        <v>0.30465300000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -861,8 +906,11 @@
       <c r="F16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J16">
+        <v>0.34517399999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -875,8 +923,11 @@
       <c r="F17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J17">
+        <v>0.35521200000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -889,8 +940,11 @@
       <c r="F18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J18">
+        <v>0.41195700000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -903,8 +957,11 @@
       <c r="F19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J19">
+        <v>1.281973</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -917,8 +974,11 @@
       <c r="F20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J20">
+        <v>3.5337139999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -931,8 +991,11 @@
       <c r="F21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J21">
+        <v>7.0253050000000004</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -945,8 +1008,11 @@
       <c r="F22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J22">
+        <v>11.482977</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -959,8 +1025,11 @@
       <c r="F23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J23">
+        <v>15.915955</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -973,8 +1042,11 @@
       <c r="F24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J24">
+        <v>19.470908999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -987,8 +1059,11 @@
       <c r="F25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J25">
+        <v>21.038800999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>5</v>
       </c>
@@ -1001,8 +1076,11 @@
       <c r="F26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J26">
+        <v>21.472373999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>17</v>
       </c>
@@ -1015,8 +1093,11 @@
       <c r="F27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J27">
+        <v>21.142890999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>18</v>
       </c>
@@ -1029,8 +1110,11 @@
       <c r="F28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J28">
+        <v>18.735417999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>19</v>
       </c>
@@ -1043,8 +1127,11 @@
       <c r="F29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J29">
+        <v>13.357785</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>5</v>
       </c>
@@ -1057,8 +1144,11 @@
       <c r="F30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J30">
+        <v>6.4831529999999997</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>2</v>
       </c>
@@ -1071,8 +1161,11 @@
       <c r="F31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J31">
+        <v>1.785272</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>20</v>
       </c>
@@ -1085,8 +1178,11 @@
       <c r="F32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J32">
+        <v>1.183E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>21</v>
       </c>
@@ -1099,8 +1195,11 @@
       <c r="F33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J33">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -1113,8 +1212,11 @@
       <c r="F34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J34">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>1</v>
       </c>
@@ -1127,8 +1229,11 @@
       <c r="F35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J35">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -1141,8 +1246,11 @@
       <c r="F36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J36">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>15</v>
       </c>
@@ -1155,8 +1263,11 @@
       <c r="F37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J37">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>23</v>
       </c>
@@ -1169,8 +1280,11 @@
       <c r="F38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J38">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>23</v>
       </c>
@@ -1183,8 +1297,11 @@
       <c r="F39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J39">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>15</v>
       </c>
@@ -1197,8 +1314,11 @@
       <c r="F40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J40">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>24</v>
       </c>
@@ -1211,8 +1331,11 @@
       <c r="F41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J41">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>25</v>
       </c>
@@ -1225,8 +1348,11 @@
       <c r="F42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J42">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>26</v>
       </c>
@@ -1239,8 +1365,11 @@
       <c r="F43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J43">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>27</v>
       </c>
@@ -1253,8 +1382,11 @@
       <c r="F44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J44">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>15</v>
       </c>
@@ -1267,8 +1399,11 @@
       <c r="F45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J45">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>6</v>
       </c>
@@ -1281,8 +1416,11 @@
       <c r="F46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J46">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>10</v>
       </c>
@@ -1295,8 +1433,11 @@
       <c r="F47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J47">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>15</v>
       </c>
@@ -1309,8 +1450,11 @@
       <c r="F48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J48">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>1</v>
       </c>
@@ -1323,8 +1467,11 @@
       <c r="F49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J49">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>15</v>
       </c>
@@ -1337,8 +1484,11 @@
       <c r="F50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J50">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>15</v>
       </c>
@@ -1351,8 +1501,11 @@
       <c r="F51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J51">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>28</v>
       </c>
@@ -1365,8 +1518,11 @@
       <c r="F52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J52">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>29</v>
       </c>
@@ -1379,8 +1535,11 @@
       <c r="F53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J53">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>30</v>
       </c>
@@ -1393,8 +1552,11 @@
       <c r="F54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J54">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>31</v>
       </c>
@@ -1407,8 +1569,11 @@
       <c r="F55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J55">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>32</v>
       </c>
@@ -1421,8 +1586,11 @@
       <c r="F56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J56">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>33</v>
       </c>
@@ -1435,8 +1603,11 @@
       <c r="F57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J57">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>34</v>
       </c>
@@ -1449,8 +1620,11 @@
       <c r="F58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J58">
+        <v>0.16202800000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>35</v>
       </c>
@@ -1463,8 +1637,11 @@
       <c r="F59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J59">
+        <v>1.776864</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>36</v>
       </c>
@@ -1477,8 +1654,11 @@
       <c r="F60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J60">
+        <v>6.0949090000000004</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>17</v>
       </c>
@@ -1491,8 +1671,11 @@
       <c r="F61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J61">
+        <v>12.074595</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>10</v>
       </c>
@@ -1505,8 +1688,11 @@
       <c r="F62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J62">
+        <v>17.063723</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>37</v>
       </c>
@@ -1519,8 +1705,11 @@
       <c r="F63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J63">
+        <v>19.815843999999998</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>15</v>
       </c>
@@ -1533,8 +1722,11 @@
       <c r="F64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J64">
+        <v>20.9209</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>15</v>
       </c>
@@ -1547,8 +1739,11 @@
       <c r="F65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J65">
+        <v>21.339689</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>17</v>
       </c>
@@ -1561,8 +1756,11 @@
       <c r="F66">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J66">
+        <v>21.447899</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>10</v>
       </c>
@@ -1575,8 +1773,11 @@
       <c r="F67">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J67">
+        <v>21.186195000000001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>28</v>
       </c>
@@ -1589,8 +1790,11 @@
       <c r="F68">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J68">
+        <v>19.166654999999999</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>38</v>
       </c>
@@ -1603,8 +1807,11 @@
       <c r="F69">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J69">
+        <v>14.146863</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>39</v>
       </c>
@@ -1617,8 +1824,11 @@
       <c r="F70">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J70">
+        <v>7.2496049999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>35</v>
       </c>
@@ -1631,8 +1841,11 @@
       <c r="F71">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J71">
+        <v>2.182194</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>40</v>
       </c>
@@ -1645,8 +1858,11 @@
       <c r="F72">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J72">
+        <v>0.107652</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>41</v>
       </c>
@@ -1659,8 +1875,11 @@
       <c r="F73">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J73">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>42</v>
       </c>
@@ -1673,8 +1892,11 @@
       <c r="F74">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J74">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>43</v>
       </c>
@@ -1687,8 +1909,11 @@
       <c r="F75">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J75">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>28</v>
       </c>
@@ -1701,8 +1926,11 @@
       <c r="F76">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J76">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>6</v>
       </c>
@@ -1715,8 +1943,11 @@
       <c r="F77">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J77">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>6</v>
       </c>
@@ -1729,8 +1960,11 @@
       <c r="F78">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J78">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>15</v>
       </c>
@@ -1743,8 +1977,11 @@
       <c r="F79">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J79">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>6</v>
       </c>
@@ -1757,8 +1994,11 @@
       <c r="F80">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J80">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>17</v>
       </c>
@@ -1771,8 +2011,11 @@
       <c r="F81">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J81">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>23</v>
       </c>
@@ -1785,8 +2028,11 @@
       <c r="F82">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J82">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>10</v>
       </c>
@@ -1799,8 +2045,11 @@
       <c r="F83">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J83">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>17</v>
       </c>
@@ -1813,8 +2062,11 @@
       <c r="F84">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J84">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>44</v>
       </c>
@@ -1827,8 +2079,11 @@
       <c r="F85">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J85">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>40</v>
       </c>
@@ -1841,8 +2096,11 @@
       <c r="F86">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J86">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>25</v>
       </c>
@@ -1855,8 +2113,11 @@
       <c r="F87">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J87">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>6</v>
       </c>
@@ -1869,8 +2130,11 @@
       <c r="F88">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J88">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>26</v>
       </c>
@@ -1883,8 +2147,11 @@
       <c r="F89">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J89">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>25</v>
       </c>
@@ -1897,8 +2164,11 @@
       <c r="F90">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J90">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>18</v>
       </c>
@@ -1911,8 +2181,11 @@
       <c r="F91">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J91">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>45</v>
       </c>
@@ -1925,8 +2198,11 @@
       <c r="F92">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J92">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>23</v>
       </c>
@@ -1939,8 +2215,11 @@
       <c r="F93">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J93">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>2</v>
       </c>
@@ -1953,8 +2232,11 @@
       <c r="F94">
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J94">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>23</v>
       </c>
@@ -1967,8 +2249,11 @@
       <c r="F95">
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J95">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>1</v>
       </c>
@@ -1981,8 +2266,11 @@
       <c r="F96">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J96">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>1</v>
       </c>
@@ -1995,8 +2283,11 @@
       <c r="F97">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J97">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>1</v>
       </c>
@@ -2009,8 +2300,11 @@
       <c r="F98">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J98">
+        <v>0.23269500000000001</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>23</v>
       </c>
@@ -2023,8 +2317,11 @@
       <c r="F99">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J99">
+        <v>2.177184</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>1</v>
       </c>
@@ -2037,8 +2334,11 @@
       <c r="F100">
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J100">
+        <v>7.3431050000000004</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>46</v>
       </c>
@@ -2051,8 +2351,11 @@
       <c r="F101">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J101">
+        <v>14.383863</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>47</v>
       </c>
@@ -2065,8 +2368,11 @@
       <c r="F102">
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J102">
+        <v>19.529909</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>46</v>
       </c>
@@ -2079,8 +2385,11 @@
       <c r="F103">
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J103">
+        <v>21.463308000000001</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>39</v>
       </c>
@@ -2093,8 +2402,11 @@
       <c r="F104">
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J104">
+        <v>21.435224999999999</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>26</v>
       </c>
@@ -2107,8 +2419,11 @@
       <c r="F105">
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J105">
+        <v>21.408878000000001</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>48</v>
       </c>
@@ -2121,8 +2436,11 @@
       <c r="F106">
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J106">
+        <v>21.42745</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>49</v>
       </c>
@@ -2135,8 +2453,11 @@
       <c r="F107">
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J107">
+        <v>21.282356</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>50</v>
       </c>
@@ -2149,8 +2470,11 @@
       <c r="F108">
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J108">
+        <v>20.056249999999999</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>17</v>
       </c>
@@ -2163,8 +2487,11 @@
       <c r="F109">
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J109">
+        <v>16.181146999999999</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>15</v>
       </c>
@@ -2177,8 +2504,11 @@
       <c r="F110">
         <v>0</v>
       </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J110">
+        <v>10.098979</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>15</v>
       </c>
@@ -2191,8 +2521,11 @@
       <c r="F111">
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J111">
+        <v>4.7711370000000004</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>2</v>
       </c>
@@ -2205,8 +2538,11 @@
       <c r="F112">
         <v>0</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J112">
+        <v>1.7305809999999999</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>28</v>
       </c>
@@ -2219,8 +2555,11 @@
       <c r="F113">
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J113">
+        <v>0.67067900000000003</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>6</v>
       </c>
@@ -2233,8 +2572,11 @@
       <c r="F114">
         <v>0</v>
       </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J114">
+        <v>0.167735</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>28</v>
       </c>
@@ -2247,8 +2589,11 @@
       <c r="F115">
         <v>0</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J115">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>6</v>
       </c>
@@ -2261,8 +2606,11 @@
       <c r="F116">
         <v>0</v>
       </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J116">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>28</v>
       </c>
@@ -2275,8 +2623,11 @@
       <c r="F117">
         <v>0</v>
       </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J117">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>51</v>
       </c>
@@ -2289,8 +2640,11 @@
       <c r="F118">
         <v>0</v>
       </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J118">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>52</v>
       </c>
@@ -2303,8 +2657,11 @@
       <c r="F119">
         <v>0</v>
       </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J119">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>53</v>
       </c>
@@ -2317,8 +2674,11 @@
       <c r="F120">
         <v>0</v>
       </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J120">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>28</v>
       </c>
@@ -2331,8 +2691,11 @@
       <c r="F121">
         <v>0</v>
       </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J121">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>23</v>
       </c>
@@ -2345,8 +2708,11 @@
       <c r="F122">
         <v>0</v>
       </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J122">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>25</v>
       </c>
@@ -2359,8 +2725,11 @@
       <c r="F123">
         <v>0</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J123">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>51</v>
       </c>
@@ -2373,8 +2742,11 @@
       <c r="F124">
         <v>0</v>
       </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J124">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>2</v>
       </c>
@@ -2387,8 +2759,11 @@
       <c r="F125">
         <v>0</v>
       </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J125">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>6</v>
       </c>
@@ -2401,8 +2776,11 @@
       <c r="F126">
         <v>0</v>
       </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J126">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>15</v>
       </c>
@@ -2415,8 +2793,11 @@
       <c r="F127">
         <v>0</v>
       </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J127">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>2</v>
       </c>
@@ -2429,8 +2810,11 @@
       <c r="F128">
         <v>0</v>
       </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J128">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>28</v>
       </c>
@@ -2443,8 +2827,11 @@
       <c r="F129">
         <v>0</v>
       </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J129">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>2</v>
       </c>
@@ -2457,8 +2844,11 @@
       <c r="F130">
         <v>0</v>
       </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J130">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>23</v>
       </c>
@@ -2471,8 +2861,11 @@
       <c r="F131">
         <v>0</v>
       </c>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J131">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>10</v>
       </c>
@@ -2485,8 +2878,11 @@
       <c r="F132">
         <v>0</v>
       </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J132">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>28</v>
       </c>
@@ -2499,8 +2895,11 @@
       <c r="F133">
         <v>0</v>
       </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J133">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>17</v>
       </c>
@@ -2513,8 +2912,11 @@
       <c r="F134">
         <v>0</v>
       </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J134">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>48</v>
       </c>
@@ -2527,8 +2929,11 @@
       <c r="F135">
         <v>0</v>
       </c>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J135">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>50</v>
       </c>
@@ -2541,8 +2946,11 @@
       <c r="F136">
         <v>0</v>
       </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J136">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>54</v>
       </c>
@@ -2555,8 +2963,11 @@
       <c r="F137">
         <v>0</v>
       </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J137">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>55</v>
       </c>
@@ -2569,8 +2980,11 @@
       <c r="F138">
         <v>0</v>
       </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J138">
+        <v>0.23269500000000001</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>1</v>
       </c>
@@ -2583,8 +2997,11 @@
       <c r="F139">
         <v>0</v>
       </c>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J139">
+        <v>2.1380050000000002</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>55</v>
       </c>
@@ -2597,8 +3014,11 @@
       <c r="F140">
         <v>0</v>
       </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J140">
+        <v>7.2104010000000001</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>1</v>
       </c>
@@ -2611,8 +3031,11 @@
       <c r="F141">
         <v>0</v>
       </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J141">
+        <v>14.240168000000001</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>15</v>
       </c>
@@ -2625,8 +3048,11 @@
       <c r="F142">
         <v>0</v>
       </c>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J142">
+        <v>19.429746999999999</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>15</v>
       </c>
@@ -2639,8 +3065,11 @@
       <c r="F143">
         <v>0</v>
       </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J143">
+        <v>21.461566999999999</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>1</v>
       </c>
@@ -2653,8 +3082,11 @@
       <c r="F144">
         <v>0</v>
       </c>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J144">
+        <v>21.438614000000001</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>28</v>
       </c>
@@ -2667,8 +3099,11 @@
       <c r="F145">
         <v>0</v>
       </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J145">
+        <v>21.416640999999998</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>15</v>
       </c>
@@ -2681,8 +3116,11 @@
       <c r="F146">
         <v>0</v>
       </c>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J146">
+        <v>21.43816</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>2</v>
       </c>
@@ -2695,8 +3133,11 @@
       <c r="F147">
         <v>0</v>
       </c>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J147">
+        <v>21.384488999999999</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>37</v>
       </c>
@@ -2709,8 +3150,11 @@
       <c r="F148">
         <v>0</v>
       </c>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J148">
+        <v>20.932922000000001</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>54</v>
       </c>
@@ -2723,8 +3167,11 @@
       <c r="F149">
         <v>0</v>
       </c>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J149">
+        <v>18.858677</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>56</v>
       </c>
@@ -2737,8 +3184,11 @@
       <c r="F150">
         <v>0</v>
       </c>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J150">
+        <v>14.983546</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>37</v>
       </c>
@@ -2751,8 +3201,11 @@
       <c r="F151">
         <v>0</v>
       </c>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J151">
+        <v>10.713836000000001</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>56</v>
       </c>
@@ -2765,8 +3218,11 @@
       <c r="F152">
         <v>0</v>
       </c>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J152">
+        <v>6.7571320000000004</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>57</v>
       </c>
@@ -2779,8 +3235,11 @@
       <c r="F153">
         <v>0</v>
       </c>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J153">
+        <v>3.5052379999999999</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>39</v>
       </c>
@@ -2793,8 +3252,11 @@
       <c r="F154">
         <v>0</v>
       </c>
-    </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J154">
+        <v>1.1518759999999999</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>25</v>
       </c>
@@ -2807,8 +3269,11 @@
       <c r="F155">
         <v>0</v>
       </c>
-    </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J155">
+        <v>0.125329</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>26</v>
       </c>
@@ -2821,8 +3286,11 @@
       <c r="F156">
         <v>0</v>
       </c>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J156">
+        <v>2.3823E-2</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>1</v>
       </c>
@@ -2835,8 +3303,11 @@
       <c r="F157">
         <v>0</v>
       </c>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J157">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>28</v>
       </c>
@@ -2849,8 +3320,11 @@
       <c r="F158">
         <v>0</v>
       </c>
-    </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J158">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>17</v>
       </c>
@@ -2863,8 +3337,11 @@
       <c r="F159">
         <v>0</v>
       </c>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J159">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>10</v>
       </c>
@@ -2877,8 +3354,11 @@
       <c r="F160">
         <v>0</v>
       </c>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J160">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>17</v>
       </c>
@@ -2891,8 +3371,11 @@
       <c r="F161">
         <v>0</v>
       </c>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J161">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>28</v>
       </c>
@@ -2905,8 +3388,11 @@
       <c r="F162">
         <v>0</v>
       </c>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J162">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>17</v>
       </c>
@@ -2919,8 +3405,11 @@
       <c r="F163">
         <v>0</v>
       </c>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J163">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>37</v>
       </c>
@@ -2933,8 +3422,11 @@
       <c r="F164">
         <v>0</v>
       </c>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J164">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>58</v>
       </c>
@@ -2947,8 +3439,11 @@
       <c r="F165">
         <v>0</v>
       </c>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J165">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>48</v>
       </c>
@@ -2961,8 +3456,11 @@
       <c r="F166">
         <v>0</v>
       </c>
-    </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J166">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>53</v>
       </c>
@@ -2975,8 +3473,11 @@
       <c r="F167">
         <v>0</v>
       </c>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J167">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>25</v>
       </c>
@@ -2989,8 +3490,11 @@
       <c r="F168">
         <v>0</v>
       </c>
-    </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J168">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>57</v>
       </c>
@@ -3003,8 +3507,11 @@
       <c r="F169">
         <v>0</v>
       </c>
-    </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J169">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>46</v>
       </c>
@@ -3017,8 +3524,11 @@
       <c r="F170">
         <v>0</v>
       </c>
-    </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J170">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>46</v>
       </c>
@@ -3031,8 +3541,11 @@
       <c r="F171">
         <v>0</v>
       </c>
-    </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J171">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>18</v>
       </c>
@@ -3045,8 +3558,11 @@
       <c r="F172">
         <v>0</v>
       </c>
-    </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J172">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>17</v>
       </c>
@@ -3059,8 +3575,11 @@
       <c r="F173">
         <v>0</v>
       </c>
-    </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J173">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>23</v>
       </c>
@@ -3073,8 +3592,11 @@
       <c r="F174">
         <v>0</v>
       </c>
-    </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J174">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>10</v>
       </c>
@@ -3087,8 +3609,11 @@
       <c r="F175">
         <v>0</v>
       </c>
-    </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J175">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>15</v>
       </c>
@@ -3101,8 +3626,11 @@
       <c r="F176">
         <v>0</v>
       </c>
-    </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J176">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>17</v>
       </c>
@@ -3115,8 +3643,11 @@
       <c r="F177">
         <v>0</v>
       </c>
-    </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J177">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>23</v>
       </c>
@@ -3129,8 +3660,11 @@
       <c r="F178">
         <v>0</v>
       </c>
-    </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J178">
+        <v>0.23269500000000001</v>
+      </c>
+    </row>
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>37</v>
       </c>
@@ -3143,8 +3677,11 @@
       <c r="F179">
         <v>0</v>
       </c>
-    </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J179">
+        <v>2.1433580000000001</v>
+      </c>
+    </row>
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>6</v>
       </c>
@@ -3157,8 +3694,11 @@
       <c r="F180">
         <v>0</v>
       </c>
-    </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J180">
+        <v>7.2438890000000002</v>
+      </c>
+    </row>
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>57</v>
       </c>
@@ -3171,8 +3711,11 @@
       <c r="F181">
         <v>0</v>
       </c>
-    </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J181">
+        <v>14.263387</v>
+      </c>
+    </row>
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>47</v>
       </c>
@@ -3185,8 +3728,11 @@
       <c r="F182">
         <v>0</v>
       </c>
-    </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J182">
+        <v>19.441593000000001</v>
+      </c>
+    </row>
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>30</v>
       </c>
@@ -3199,8 +3745,11 @@
       <c r="F183">
         <v>0</v>
       </c>
-    </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J183">
+        <v>21.474246999999998</v>
+      </c>
+    </row>
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>47</v>
       </c>
@@ -3213,8 +3762,11 @@
       <c r="F184">
         <v>0</v>
       </c>
-    </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J184">
+        <v>21.463837000000002</v>
+      </c>
+    </row>
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>15</v>
       </c>
@@ -3227,8 +3779,11 @@
       <c r="F185">
         <v>0</v>
       </c>
-    </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J185">
+        <v>21.453796000000001</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>9</v>
       </c>
@@ -3241,8 +3796,11 @@
       <c r="F186">
         <v>0</v>
       </c>
-    </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J186">
+        <v>21.462630999999998</v>
+      </c>
+    </row>
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>59</v>
       </c>
@@ -3255,8 +3813,11 @@
       <c r="F187">
         <v>0</v>
       </c>
-    </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J187">
+        <v>21.442696000000002</v>
+      </c>
+    </row>
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>37</v>
       </c>
@@ -3269,8 +3830,11 @@
       <c r="F188">
         <v>0</v>
       </c>
-    </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J188">
+        <v>21.352557999999998</v>
+      </c>
+    </row>
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>37</v>
       </c>
@@ -3283,8 +3847,11 @@
       <c r="F189">
         <v>0</v>
       </c>
-    </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J189">
+        <v>20.747602000000001</v>
+      </c>
+    </row>
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>2</v>
       </c>
@@ -3297,8 +3864,11 @@
       <c r="F190">
         <v>0</v>
       </c>
-    </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J190">
+        <v>19.383524000000001</v>
+      </c>
+    </row>
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>37</v>
       </c>
@@ -3311,8 +3881,11 @@
       <c r="F191">
         <v>0</v>
       </c>
-    </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J191">
+        <v>17.409890999999998</v>
+      </c>
+    </row>
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>45</v>
       </c>
@@ -3325,8 +3898,11 @@
       <c r="F192">
         <v>0</v>
       </c>
-    </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J192">
+        <v>13.968514000000001</v>
+      </c>
+    </row>
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>17</v>
       </c>
@@ -3339,8 +3915,11 @@
       <c r="F193">
         <v>0</v>
       </c>
-    </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J193">
+        <v>9.1633689999999994</v>
+      </c>
+    </row>
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>5</v>
       </c>
@@ -3353,8 +3932,11 @@
       <c r="F194">
         <v>0</v>
       </c>
-    </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J194">
+        <v>4.2175209999999996</v>
+      </c>
+    </row>
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>6</v>
       </c>
@@ -3367,8 +3949,11 @@
       <c r="F195">
         <v>0</v>
       </c>
-    </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J195">
+        <v>1.1498569999999999</v>
+      </c>
+    </row>
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>6</v>
       </c>
@@ -3381,8 +3966,11 @@
       <c r="F196">
         <v>0</v>
       </c>
-    </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J196">
+        <v>0.228828</v>
+      </c>
+    </row>
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>5</v>
       </c>
@@ -3395,8 +3983,11 @@
       <c r="F197">
         <v>0</v>
       </c>
-    </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J197">
+        <v>1.183E-2</v>
+      </c>
+    </row>
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>60</v>
       </c>
@@ -3409,8 +4000,11 @@
       <c r="F198">
         <v>0</v>
       </c>
-    </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J198">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>5</v>
       </c>
@@ -3423,8 +4017,11 @@
       <c r="F199">
         <v>0</v>
       </c>
-    </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J199">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>5</v>
       </c>
@@ -3437,8 +4034,11 @@
       <c r="F200">
         <v>0</v>
       </c>
-    </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J200">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>15</v>
       </c>
@@ -3451,8 +4051,11 @@
       <c r="F201">
         <v>0</v>
       </c>
-    </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J201">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>28</v>
       </c>
@@ -3465,8 +4068,11 @@
       <c r="F202">
         <v>0</v>
       </c>
-    </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J202">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>45</v>
       </c>
@@ -3479,8 +4085,11 @@
       <c r="F203">
         <v>0</v>
       </c>
-    </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J203">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>9</v>
       </c>
@@ -3493,8 +4102,11 @@
       <c r="F204">
         <v>0</v>
       </c>
-    </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J204">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>23</v>
       </c>
@@ -3507,8 +4119,11 @@
       <c r="F205">
         <v>0</v>
       </c>
-    </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J205">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>17</v>
       </c>
@@ -3521,8 +4136,11 @@
       <c r="F206">
         <v>0</v>
       </c>
-    </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J206">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>6</v>
       </c>
@@ -3535,8 +4153,11 @@
       <c r="F207">
         <v>0</v>
       </c>
-    </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J207">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>36</v>
       </c>
@@ -3549,8 +4170,11 @@
       <c r="F208">
         <v>0</v>
       </c>
-    </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J208">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>6</v>
       </c>
@@ -3563,8 +4187,11 @@
       <c r="F209">
         <v>0</v>
       </c>
-    </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J209">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>5</v>
       </c>
@@ -3577,8 +4204,11 @@
       <c r="F210">
         <v>0</v>
       </c>
-    </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J210">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>17</v>
       </c>
@@ -3591,8 +4221,11 @@
       <c r="F211">
         <v>0</v>
       </c>
-    </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J211">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>1</v>
       </c>
@@ -3605,8 +4238,11 @@
       <c r="F212">
         <v>0</v>
       </c>
-    </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J212">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>1</v>
       </c>
@@ -3619,8 +4255,11 @@
       <c r="F213">
         <v>0</v>
       </c>
-    </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J213">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>10</v>
       </c>
@@ -3633,8 +4272,11 @@
       <c r="F214">
         <v>0</v>
       </c>
-    </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J214">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>6</v>
       </c>
@@ -3647,8 +4289,11 @@
       <c r="F215">
         <v>0</v>
       </c>
-    </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J215">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>2</v>
       </c>
@@ -3661,8 +4306,11 @@
       <c r="F216">
         <v>0</v>
       </c>
-    </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J216">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>37</v>
       </c>
@@ -3675,8 +4323,11 @@
       <c r="F217">
         <v>0</v>
       </c>
-    </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J217">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>59</v>
       </c>
@@ -3689,8 +4340,11 @@
       <c r="F218">
         <v>0</v>
       </c>
-    </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J218">
+        <v>0.21850800000000001</v>
+      </c>
+    </row>
+    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>23</v>
       </c>
@@ -3703,8 +4357,11 @@
       <c r="F219">
         <v>0</v>
       </c>
-    </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J219">
+        <v>2.0063460000000002</v>
+      </c>
+    </row>
+    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>23</v>
       </c>
@@ -3717,8 +4374,11 @@
       <c r="F220">
         <v>0</v>
       </c>
-    </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J220">
+        <v>6.7880070000000003</v>
+      </c>
+    </row>
+    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>2</v>
       </c>
@@ -3731,8 +4391,11 @@
       <c r="F221">
         <v>0</v>
       </c>
-    </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J221">
+        <v>13.37618</v>
+      </c>
+    </row>
+    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>2</v>
       </c>
@@ -3745,8 +4408,11 @@
       <c r="F222">
         <v>0</v>
       </c>
-    </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J222">
+        <v>18.254584999999999</v>
+      </c>
+    </row>
+    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>2</v>
       </c>
@@ -3759,8 +4425,11 @@
       <c r="F223">
         <v>0</v>
       </c>
-    </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J223">
+        <v>20.262862999999999</v>
+      </c>
+    </row>
+    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>6</v>
       </c>
@@ -3773,8 +4442,11 @@
       <c r="F224">
         <v>0</v>
       </c>
-    </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J224">
+        <v>20.492605000000001</v>
+      </c>
+    </row>
+    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>9</v>
       </c>
@@ -3787,8 +4459,11 @@
       <c r="F225">
         <v>0</v>
       </c>
-    </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J225">
+        <v>20.652958000000002</v>
+      </c>
+    </row>
+    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>37</v>
       </c>
@@ -3801,8 +4476,11 @@
       <c r="F226">
         <v>0</v>
       </c>
-    </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J226">
+        <v>20.875404</v>
+      </c>
+    </row>
+    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>15</v>
       </c>
@@ -3815,8 +4493,11 @@
       <c r="F227">
         <v>0</v>
       </c>
-    </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J227">
+        <v>21.160171999999999</v>
+      </c>
+    </row>
+    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>9</v>
       </c>
@@ -3829,8 +4510,11 @@
       <c r="F228">
         <v>0</v>
       </c>
-    </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J228">
+        <v>21.392719</v>
+      </c>
+    </row>
+    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>2</v>
       </c>
@@ -3843,8 +4527,11 @@
       <c r="F229">
         <v>0</v>
       </c>
-    </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J229">
+        <v>21.442696000000002</v>
+      </c>
+    </row>
+    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>23</v>
       </c>
@@ -3857,8 +4544,11 @@
       <c r="F230">
         <v>0</v>
       </c>
-    </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J230">
+        <v>21.304538999999998</v>
+      </c>
+    </row>
+    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>2</v>
       </c>
@@ -3871,8 +4561,11 @@
       <c r="F231">
         <v>0</v>
       </c>
-    </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J231">
+        <v>20.874466000000002</v>
+      </c>
+    </row>
+    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>15</v>
       </c>
@@ -3885,8 +4578,11 @@
       <c r="F232">
         <v>0</v>
       </c>
-    </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J232">
+        <v>19.069808999999999</v>
+      </c>
+    </row>
+    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>23</v>
       </c>
@@ -3899,8 +4595,11 @@
       <c r="F233">
         <v>0</v>
       </c>
-    </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J233">
+        <v>15.154051000000001</v>
+      </c>
+    </row>
+    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>10</v>
       </c>
@@ -3913,8 +4612,11 @@
       <c r="F234">
         <v>0</v>
       </c>
-    </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J234">
+        <v>9.0770999999999997</v>
+      </c>
+    </row>
+    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>6</v>
       </c>
@@ -3927,8 +4629,11 @@
       <c r="F235">
         <v>0</v>
       </c>
-    </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J235">
+        <v>3.7688220000000001</v>
+      </c>
+    </row>
+    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>61</v>
       </c>
@@ -3941,8 +4646,11 @@
       <c r="F236">
         <v>0</v>
       </c>
-    </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J236">
+        <v>0.86477400000000004</v>
+      </c>
+    </row>
+    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>2</v>
       </c>
@@ -3955,8 +4663,11 @@
       <c r="F237">
         <v>0</v>
       </c>
-    </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J237">
+        <v>6.3678999999999999E-2</v>
+      </c>
+    </row>
+    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>10</v>
       </c>
@@ -3969,8 +4680,11 @@
       <c r="F238">
         <v>0</v>
       </c>
-    </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J238">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>2</v>
       </c>
@@ -3983,8 +4697,11 @@
       <c r="F239">
         <v>0</v>
       </c>
-    </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J239">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>23</v>
       </c>
@@ -3997,8 +4714,11 @@
       <c r="F240">
         <v>0</v>
       </c>
-    </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J240">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>2</v>
       </c>
@@ -4011,8 +4731,11 @@
       <c r="F241">
         <v>0</v>
       </c>
-    </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J241">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>23</v>
       </c>
@@ -4025,8 +4748,11 @@
       <c r="F242">
         <v>0</v>
       </c>
-    </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J242">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>23</v>
       </c>
@@ -4039,8 +4765,11 @@
       <c r="F243">
         <v>0</v>
       </c>
-    </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J243">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>37</v>
       </c>
@@ -4053,8 +4782,11 @@
       <c r="F244">
         <v>0</v>
       </c>
-    </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J244">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>15</v>
       </c>
@@ -4067,8 +4799,11 @@
       <c r="F245">
         <v>0</v>
       </c>
-    </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J245">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>62</v>
       </c>
@@ -4081,8 +4816,11 @@
       <c r="F246">
         <v>0</v>
       </c>
-    </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J246">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>1</v>
       </c>
@@ -4095,8 +4833,11 @@
       <c r="F247">
         <v>0</v>
       </c>
-    </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J247">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>10</v>
       </c>
@@ -4109,8 +4850,11 @@
       <c r="F248">
         <v>0</v>
       </c>
-    </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J248">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>15</v>
       </c>
@@ -4123,8 +4867,11 @@
       <c r="F249">
         <v>0</v>
       </c>
-    </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J249">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>23</v>
       </c>
@@ -4137,8 +4884,11 @@
       <c r="F250">
         <v>0</v>
       </c>
-    </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J250">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>37</v>
       </c>
@@ -4151,8 +4901,11 @@
       <c r="F251">
         <v>0</v>
       </c>
-    </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J251">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>10</v>
       </c>
@@ -4165,8 +4918,11 @@
       <c r="F252">
         <v>0</v>
       </c>
-    </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J252">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>1</v>
       </c>
@@ -4179,8 +4935,11 @@
       <c r="F253">
         <v>0</v>
       </c>
-    </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J253">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>15</v>
       </c>
@@ -4193,8 +4952,11 @@
       <c r="F254">
         <v>0</v>
       </c>
-    </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J254">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>17</v>
       </c>
@@ -4207,8 +4969,11 @@
       <c r="F255">
         <v>0</v>
       </c>
-    </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J255">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>63</v>
       </c>
@@ -4221,8 +4986,11 @@
       <c r="F256">
         <v>0</v>
       </c>
-    </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J256">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>17</v>
       </c>
@@ -4235,8 +5003,11 @@
       <c r="F257">
         <v>0</v>
       </c>
-    </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J257">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>60</v>
       </c>
@@ -4249,8 +5020,11 @@
       <c r="F258">
         <v>0</v>
       </c>
-    </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J258">
+        <v>0.164772</v>
+      </c>
+    </row>
+    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>15</v>
       </c>
@@ -4263,8 +5037,11 @@
       <c r="F259">
         <v>0</v>
       </c>
-    </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J259">
+        <v>1.5142880000000001</v>
+      </c>
+    </row>
+    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>2</v>
       </c>
@@ -4277,8 +5054,11 @@
       <c r="F260">
         <v>0</v>
       </c>
-    </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J260">
+        <v>5.128107</v>
+      </c>
+    </row>
+    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>5</v>
       </c>
@@ -4291,8 +5071,11 @@
       <c r="F261">
         <v>0</v>
       </c>
-    </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J261">
+        <v>10.207819000000001</v>
+      </c>
+    </row>
+    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>61</v>
       </c>
@@ -4305,8 +5088,11 @@
       <c r="F262">
         <v>0</v>
       </c>
-    </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J262">
+        <v>13.976569</v>
+      </c>
+    </row>
+    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>28</v>
       </c>
@@ -4319,8 +5105,11 @@
       <c r="F263">
         <v>0</v>
       </c>
-    </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J263">
+        <v>15.875659000000001</v>
+      </c>
+    </row>
+    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>17</v>
       </c>
@@ -4333,8 +5122,11 @@
       <c r="F264">
         <v>0</v>
       </c>
-    </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J264">
+        <v>16.682041000000002</v>
+      </c>
+    </row>
+    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>31</v>
       </c>
@@ -4347,8 +5139,11 @@
       <c r="F265">
         <v>0</v>
       </c>
-    </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J265">
+        <v>17.3354</v>
+      </c>
+    </row>
+    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>64</v>
       </c>
@@ -4361,8 +5156,11 @@
       <c r="F266">
         <v>0</v>
       </c>
-    </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J266">
+        <v>18.202126</v>
+      </c>
+    </row>
+    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>2</v>
       </c>
@@ -4375,8 +5173,11 @@
       <c r="F267">
         <v>0</v>
       </c>
-    </row>
-    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J267">
+        <v>19.343315</v>
+      </c>
+    </row>
+    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>65</v>
       </c>
@@ -4389,8 +5190,11 @@
       <c r="F268">
         <v>0</v>
       </c>
-    </row>
-    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J268">
+        <v>20.510141000000001</v>
+      </c>
+    </row>
+    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>15</v>
       </c>
@@ -4403,8 +5207,11 @@
       <c r="F269">
         <v>0</v>
       </c>
-    </row>
-    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J269">
+        <v>21.132695999999999</v>
+      </c>
+    </row>
+    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>15</v>
       </c>
@@ -4417,8 +5224,11 @@
       <c r="F270">
         <v>0</v>
       </c>
-    </row>
-    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J270">
+        <v>21.326212000000002</v>
+      </c>
+    </row>
+    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>66</v>
       </c>
@@ -4431,8 +5241,11 @@
       <c r="F271">
         <v>0</v>
       </c>
-    </row>
-    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J271">
+        <v>21.379390999999998</v>
+      </c>
+    </row>
+    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>36</v>
       </c>
@@ -4445,8 +5258,11 @@
       <c r="F272">
         <v>0</v>
       </c>
-    </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J272">
+        <v>20.971043000000002</v>
+      </c>
+    </row>
+    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>31</v>
       </c>
@@ -4459,8 +5275,11 @@
       <c r="F273">
         <v>0</v>
       </c>
-    </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J273">
+        <v>19.157284000000001</v>
+      </c>
+    </row>
+    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>31</v>
       </c>
@@ -4473,8 +5292,11 @@
       <c r="F274">
         <v>0</v>
       </c>
-    </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J274">
+        <v>13.827256</v>
+      </c>
+    </row>
+    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>45</v>
       </c>
@@ -4487,8 +5309,11 @@
       <c r="F275">
         <v>0</v>
       </c>
-    </row>
-    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J275">
+        <v>7.2816770000000002</v>
+      </c>
+    </row>
+    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>67</v>
       </c>
@@ -4501,8 +5326,11 @@
       <c r="F276">
         <v>0</v>
       </c>
-    </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J276">
+        <v>2.0797150000000002</v>
+      </c>
+    </row>
+    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>23</v>
       </c>
@@ -4515,8 +5343,11 @@
       <c r="F277">
         <v>0</v>
       </c>
-    </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J277">
+        <v>0.28721200000000002</v>
+      </c>
+    </row>
+    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>68</v>
       </c>
@@ -4529,8 +5360,11 @@
       <c r="F278">
         <v>0</v>
       </c>
-    </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J278">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>6</v>
       </c>
@@ -4543,8 +5377,11 @@
       <c r="F279">
         <v>0</v>
       </c>
-    </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J279">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>6</v>
       </c>
@@ -4557,8 +5394,11 @@
       <c r="F280">
         <v>0</v>
       </c>
-    </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J280">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>2</v>
       </c>
@@ -4571,8 +5411,11 @@
       <c r="F281">
         <v>0</v>
       </c>
-    </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J281">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>31</v>
       </c>
@@ -4585,8 +5428,11 @@
       <c r="F282">
         <v>0</v>
       </c>
-    </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J282">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>28</v>
       </c>
@@ -4599,8 +5445,11 @@
       <c r="F283">
         <v>0</v>
       </c>
-    </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J283">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>64</v>
       </c>
@@ -4613,8 +5462,11 @@
       <c r="F284">
         <v>0</v>
       </c>
-    </row>
-    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J284">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>59</v>
       </c>
@@ -4627,8 +5479,11 @@
       <c r="F285">
         <v>0</v>
       </c>
-    </row>
-    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J285">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>43</v>
       </c>
@@ -4641,8 +5496,11 @@
       <c r="F286">
         <v>0</v>
       </c>
-    </row>
-    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J286">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>37</v>
       </c>
@@ -4655,8 +5513,11 @@
       <c r="F287">
         <v>0</v>
       </c>
-    </row>
-    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J287">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>63</v>
       </c>
@@ -4669,8 +5530,11 @@
       <c r="F288">
         <v>0</v>
       </c>
-    </row>
-    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J288">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>10</v>
       </c>
@@ -4683,8 +5547,11 @@
       <c r="F289">
         <v>0</v>
       </c>
-    </row>
-    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J289">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="290" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>23</v>
       </c>
@@ -4697,8 +5564,11 @@
       <c r="F290">
         <v>0</v>
       </c>
-    </row>
-    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J290">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="291" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>17</v>
       </c>
@@ -4711,8 +5581,11 @@
       <c r="F291">
         <v>0</v>
       </c>
-    </row>
-    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J291">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="292" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>31</v>
       </c>
@@ -4725,8 +5598,11 @@
       <c r="F292">
         <v>0</v>
       </c>
-    </row>
-    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J292">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="293" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>6</v>
       </c>
@@ -4739,8 +5615,11 @@
       <c r="F293">
         <v>0</v>
       </c>
-    </row>
-    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J293">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="294" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>66</v>
       </c>
@@ -4753,8 +5632,11 @@
       <c r="F294">
         <v>0</v>
       </c>
-    </row>
-    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J294">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>66</v>
       </c>
@@ -4767,8 +5649,11 @@
       <c r="F295">
         <v>0</v>
       </c>
-    </row>
-    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J295">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="296" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>34</v>
       </c>
@@ -4781,8 +5666,11 @@
       <c r="F296">
         <v>0</v>
       </c>
-    </row>
-    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J296">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="297" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>37</v>
       </c>
@@ -4795,8 +5683,11 @@
       <c r="F297">
         <v>0</v>
       </c>
-    </row>
-    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J297">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="298" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>61</v>
       </c>
@@ -4809,8 +5700,11 @@
       <c r="F298">
         <v>0</v>
       </c>
-    </row>
-    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J298">
+        <v>8.2195000000000004E-2</v>
+      </c>
+    </row>
+    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>5</v>
       </c>
@@ -4823,8 +5717,11 @@
       <c r="F299">
         <v>0</v>
       </c>
-    </row>
-    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J299">
+        <v>0.78143399999999996</v>
+      </c>
+    </row>
+    <row r="300" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>63</v>
       </c>
@@ -4837,8 +5734,11 @@
       <c r="F300">
         <v>0</v>
       </c>
-    </row>
-    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J300">
+        <v>2.6398160000000002</v>
+      </c>
+    </row>
+    <row r="301" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>1</v>
       </c>
@@ -4851,8 +5751,11 @@
       <c r="F301">
         <v>0</v>
       </c>
-    </row>
-    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J301">
+        <v>5.3458949999999996</v>
+      </c>
+    </row>
+    <row r="302" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>1</v>
       </c>
@@ -4865,8 +5768,11 @@
       <c r="F302">
         <v>0</v>
       </c>
-    </row>
-    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J302">
+        <v>7.3450600000000001</v>
+      </c>
+    </row>
+    <row r="303" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>23</v>
       </c>
@@ -4879,8 +5785,11 @@
       <c r="F303">
         <v>7.8429999999999993E-3</v>
       </c>
-    </row>
-    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J303">
+        <v>8.7439990000000005</v>
+      </c>
+    </row>
+    <row r="304" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>10</v>
       </c>
@@ -4893,8 +5802,11 @@
       <c r="F304">
         <v>5.8824000000000001E-2</v>
       </c>
-    </row>
-    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J304">
+        <v>9.8795129999999993</v>
+      </c>
+    </row>
+    <row r="305" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>36</v>
       </c>
@@ -4907,8 +5819,11 @@
       <c r="F305">
         <v>8.2352999999999996E-2</v>
       </c>
-    </row>
-    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J305">
+        <v>10.941658</v>
+      </c>
+    </row>
+    <row r="306" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>45</v>
       </c>
@@ -4921,8 +5836,11 @@
       <c r="F306">
         <v>8.6275000000000004E-2</v>
       </c>
-    </row>
-    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J306">
+        <v>12.216100000000001</v>
+      </c>
+    </row>
+    <row r="307" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>15</v>
       </c>
@@ -4935,8 +5853,11 @@
       <c r="F307">
         <v>8.2352999999999996E-2</v>
       </c>
-    </row>
-    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J307">
+        <v>13.95185</v>
+      </c>
+    </row>
+    <row r="308" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>37</v>
       </c>
@@ -4949,8 +5870,11 @@
       <c r="F308">
         <v>8.6275000000000004E-2</v>
       </c>
-    </row>
-    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J308">
+        <v>16.332380000000001</v>
+      </c>
+    </row>
+    <row r="309" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>37</v>
       </c>
@@ -4963,8 +5887,11 @@
       <c r="F309">
         <v>0.15294099999999999</v>
       </c>
-    </row>
-    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J309">
+        <v>18.524222999999999</v>
+      </c>
+    </row>
+    <row r="310" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>36</v>
       </c>
@@ -4977,8 +5904,11 @@
       <c r="F310">
         <v>0.34902</v>
       </c>
-    </row>
-    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J310">
+        <v>20.157976000000001</v>
+      </c>
+    </row>
+    <row r="311" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>2</v>
       </c>
@@ -4991,8 +5921,11 @@
       <c r="F311">
         <v>0.23921600000000001</v>
       </c>
-    </row>
-    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J311">
+        <v>21.135079999999999</v>
+      </c>
+    </row>
+    <row r="312" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>2</v>
       </c>
@@ -5005,8 +5938,11 @@
       <c r="F312">
         <v>7.0587999999999998E-2</v>
       </c>
-    </row>
-    <row r="313" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J312">
+        <v>21.426376000000001</v>
+      </c>
+    </row>
+    <row r="313" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>37</v>
       </c>
@@ -5019,8 +5955,11 @@
       <c r="F313">
         <v>8.2352999999999996E-2</v>
       </c>
-    </row>
-    <row r="314" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J313">
+        <v>20.774768999999999</v>
+      </c>
+    </row>
+    <row r="314" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>37</v>
       </c>
@@ -5033,8 +5972,11 @@
       <c r="F314">
         <v>9.0195999999999998E-2</v>
       </c>
-    </row>
-    <row r="315" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J314">
+        <v>17.220141999999999</v>
+      </c>
+    </row>
+    <row r="315" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>62</v>
       </c>
@@ -5047,8 +5989,11 @@
       <c r="F315">
         <v>7.4510000000000007E-2</v>
       </c>
-    </row>
-    <row r="316" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J315">
+        <v>11.090724</v>
+      </c>
+    </row>
+    <row r="316" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>17</v>
       </c>
@@ -5061,8 +6006,11 @@
       <c r="F316">
         <v>2.3529000000000001E-2</v>
       </c>
-    </row>
-    <row r="317" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J316">
+        <v>4.3875840000000004</v>
+      </c>
+    </row>
+    <row r="317" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>15</v>
       </c>
@@ -5075,8 +6023,11 @@
       <c r="F317">
         <v>0</v>
       </c>
-    </row>
-    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J317">
+        <v>0.99529500000000004</v>
+      </c>
+    </row>
+    <row r="318" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>17</v>
       </c>
@@ -5089,8 +6040,11 @@
       <c r="F318">
         <v>0</v>
       </c>
-    </row>
-    <row r="319" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J318">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="319" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>15</v>
       </c>
@@ -5103,8 +6057,11 @@
       <c r="F319">
         <v>0</v>
       </c>
-    </row>
-    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J319">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="320" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>9</v>
       </c>
@@ -5117,8 +6074,11 @@
       <c r="F320">
         <v>0</v>
       </c>
-    </row>
-    <row r="321" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J320">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="321" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>15</v>
       </c>
@@ -5131,8 +6091,11 @@
       <c r="F321">
         <v>0</v>
       </c>
-    </row>
-    <row r="322" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J321">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="322" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>15</v>
       </c>
@@ -5145,8 +6108,11 @@
       <c r="F322">
         <v>0</v>
       </c>
-    </row>
-    <row r="323" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J322">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="323" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>5</v>
       </c>
@@ -5159,8 +6125,11 @@
       <c r="F323">
         <v>0</v>
       </c>
-    </row>
-    <row r="324" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J323">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="324" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>23</v>
       </c>
@@ -5173,8 +6142,11 @@
       <c r="F324">
         <v>0</v>
       </c>
-    </row>
-    <row r="325" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J324">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="325" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>66</v>
       </c>
@@ -5187,8 +6159,11 @@
       <c r="F325">
         <v>0</v>
       </c>
-    </row>
-    <row r="326" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J325">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="326" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>2</v>
       </c>
@@ -5201,8 +6176,11 @@
       <c r="F326">
         <v>0</v>
       </c>
-    </row>
-    <row r="327" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J326">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="327" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>2</v>
       </c>
@@ -5215,8 +6193,11 @@
       <c r="F327">
         <v>0</v>
       </c>
-    </row>
-    <row r="328" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J327">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="328" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>17</v>
       </c>
@@ -5229,8 +6210,11 @@
       <c r="F328">
         <v>0</v>
       </c>
-    </row>
-    <row r="329" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J328">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="329" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>17</v>
       </c>
@@ -5243,8 +6227,11 @@
       <c r="F329">
         <v>0</v>
       </c>
-    </row>
-    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J329">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="330" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>6</v>
       </c>
@@ -5257,8 +6244,11 @@
       <c r="F330">
         <v>0</v>
       </c>
-    </row>
-    <row r="331" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J330">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="331" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>15</v>
       </c>
@@ -5271,8 +6261,11 @@
       <c r="F331">
         <v>0</v>
       </c>
-    </row>
-    <row r="332" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J331">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="332" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>15</v>
       </c>
@@ -5285,8 +6278,11 @@
       <c r="F332">
         <v>0</v>
       </c>
-    </row>
-    <row r="333" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J332">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="333" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>9</v>
       </c>
@@ -5299,8 +6295,11 @@
       <c r="F333">
         <v>0</v>
       </c>
-    </row>
-    <row r="334" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J333">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="334" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>15</v>
       </c>
@@ -5313,8 +6312,11 @@
       <c r="F334">
         <v>0</v>
       </c>
-    </row>
-    <row r="335" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J334">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="335" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>62</v>
       </c>
@@ -5327,8 +6329,11 @@
       <c r="F335">
         <v>0</v>
       </c>
-    </row>
-    <row r="336" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J335">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="336" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>2</v>
       </c>
@@ -5341,8 +6346,11 @@
       <c r="F336">
         <v>0</v>
       </c>
-    </row>
-    <row r="337" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J336">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="337" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>2</v>
       </c>
@@ -5355,8 +6363,11 @@
       <c r="F337">
         <v>0</v>
       </c>
-    </row>
-    <row r="338" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J337">
+        <v>3.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="338" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>1</v>
       </c>
@@ -5369,8 +6380,11 @@
       <c r="F338">
         <v>0</v>
       </c>
-    </row>
-    <row r="339" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J338">
+        <v>2.1500999999999999E-2</v>
+      </c>
+    </row>
+    <row r="339" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>1</v>
       </c>
@@ -5383,8 +6397,11 @@
       <c r="F339">
         <v>0</v>
       </c>
-    </row>
-    <row r="340" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J339">
+        <v>0.23936499999999999</v>
+      </c>
+    </row>
+    <row r="340" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>5</v>
       </c>
@@ -5397,8 +6414,11 @@
       <c r="F340">
         <v>0</v>
       </c>
-    </row>
-    <row r="341" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J340">
+        <v>0.80900499999999997</v>
+      </c>
+    </row>
+    <row r="341" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>23</v>
       </c>
@@ -5412,7 +6432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="342" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>23</v>
       </c>
@@ -5426,7 +6446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="343" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>15</v>
       </c>
@@ -5440,7 +6460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="344" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>2</v>
       </c>
@@ -5454,7 +6474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="345" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>62</v>
       </c>
@@ -5468,7 +6488,7 @@
         <v>3.1372999999999998E-2</v>
       </c>
     </row>
-    <row r="346" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>2</v>
       </c>
@@ -5482,7 +6502,7 @@
         <v>0.25097999999999998</v>
       </c>
     </row>
-    <row r="347" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>17</v>
       </c>
@@ -5496,7 +6516,7 @@
         <v>0.34509800000000002</v>
       </c>
     </row>
-    <row r="348" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>17</v>
       </c>
@@ -5510,7 +6530,7 @@
         <v>0.36862699999999998</v>
       </c>
     </row>
-    <row r="349" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>15</v>
       </c>
@@ -5524,7 +6544,7 @@
         <v>0.36470599999999997</v>
       </c>
     </row>
-    <row r="350" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>10</v>
       </c>
@@ -5538,7 +6558,7 @@
         <v>0.36470599999999997</v>
       </c>
     </row>
-    <row r="351" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>6</v>
       </c>
@@ -5552,7 +6572,7 @@
         <v>0.478431</v>
       </c>
     </row>
-    <row r="352" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>6</v>
       </c>

</xml_diff>